<commit_message>
xl data change commit
</commit_message>
<xml_diff>
--- a/src/test/resources/AmazonTestData.xlsx
+++ b/src/test/resources/AmazonTestData.xlsx
@@ -33,9 +33,6 @@
     <t>customer service page title</t>
   </si>
   <si>
-    <t>Amazon Customer Service Support – Amazon.com</t>
-  </si>
-  <si>
     <t>registry page title</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>https://www.amazon.com/b/?_encoding</t>
+  </si>
+  <si>
+    <t>Help &amp; Contact Us - Amazon Customer Service</t>
   </si>
 </sst>
 </file>
@@ -133,9 +133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -442,7 +443,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +462,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,10 +478,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,55 +489,56 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>